<commit_message>
Task 14 & 15 are completed
</commit_message>
<xml_diff>
--- a/SourceCode/2023/Oct2023/Basics/SachinRawal/Task1/Task14/Vajrang.xlsx
+++ b/SourceCode/2023/Oct2023/Basics/SachinRawal/Task1/Task14/Vajrang.xlsx
@@ -5680,6 +5680,1532 @@
         <x:v>12</x:v>
       </x:c>
     </x:row>
+    <x:row r="92" spans="1:4">
+      <x:c r="A92" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:4">
+      <x:c r="A93" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:4">
+      <x:c r="A94" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:4">
+      <x:c r="A95" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:4">
+      <x:c r="A96" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:4">
+      <x:c r="A97" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:4">
+      <x:c r="A98" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:4">
+      <x:c r="A99" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:4">
+      <x:c r="A100" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:4">
+      <x:c r="A101" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="C101" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="D101" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:4">
+      <x:c r="A102" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="C102" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="D102" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:4">
+      <x:c r="A103" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="C103" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="D103" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:4">
+      <x:c r="A104" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="C104" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="D104" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:4">
+      <x:c r="A105" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="C105" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="D105" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:4">
+      <x:c r="A106" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+      <x:c r="C106" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+      <x:c r="D106" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:4">
+      <x:c r="A107" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="C107" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="D107" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:4">
+      <x:c r="A108" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="C108" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="D108" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:4">
+      <x:c r="A109" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="C109" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="D109" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:4">
+      <x:c r="A110" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+      <x:c r="C110" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="D110" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:4">
+      <x:c r="A111" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="C111" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="D111" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:4">
+      <x:c r="A112" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+      <x:c r="C112" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="D112" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:4">
+      <x:c r="A113" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="C113" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="D113" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:4">
+      <x:c r="A114" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B114" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="C114" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="D114" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:4">
+      <x:c r="A115" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="C115" s="0" t="s">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="D115" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:4">
+      <x:c r="A116" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+      <x:c r="C116" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="D116" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:4">
+      <x:c r="A117" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="C117" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+      <x:c r="D117" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:4">
+      <x:c r="A118" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+      <x:c r="C118" s="0" t="s">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="D118" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:4">
+      <x:c r="A119" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+      <x:c r="C119" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+      <x:c r="D119" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:4">
+      <x:c r="A120" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="C120" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="D120" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121" spans="1:4">
+      <x:c r="A121" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B121" s="0" t="s">
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="C121" s="0" t="s">
+        <x:v>246</x:v>
+      </x:c>
+      <x:c r="D121" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122" spans="1:4">
+      <x:c r="A122" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B122" s="0" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="C122" s="0" t="s">
+        <x:v>248</x:v>
+      </x:c>
+      <x:c r="D122" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123" spans="1:4">
+      <x:c r="A123" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B123" s="0" t="s">
+        <x:v>249</x:v>
+      </x:c>
+      <x:c r="C123" s="0" t="s">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="D123" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124" spans="1:4">
+      <x:c r="A124" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="C124" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="D124" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125" spans="1:4">
+      <x:c r="A125" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B125" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="C125" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="D125" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:4">
+      <x:c r="A126" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="C126" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="D126" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:4">
+      <x:c r="A127" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="C127" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="D127" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128" spans="1:4">
+      <x:c r="A128" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B128" s="0" t="s">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="C128" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="D128" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129" spans="1:4">
+      <x:c r="A129" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B129" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="C129" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="D129" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130" spans="1:4">
+      <x:c r="A130" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B130" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="C130" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="D130" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:4">
+      <x:c r="A131" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="C131" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D131" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:4">
+      <x:c r="A132" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
+        <x:v>267</x:v>
+      </x:c>
+      <x:c r="C132" s="0" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="D132" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:4">
+      <x:c r="A133" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="C133" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="D133" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:4">
+      <x:c r="A134" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="C134" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="D134" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:4">
+      <x:c r="A135" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="C135" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="D135" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" spans="1:4">
+      <x:c r="A136" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B136" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+      <x:c r="C136" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="D136" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137" spans="1:4">
+      <x:c r="A137" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B137" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="C137" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="D137" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138" spans="1:4">
+      <x:c r="A138" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="C138" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="D138" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:4">
+      <x:c r="A139" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="C139" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="D139" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:4">
+      <x:c r="A140" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="C140" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="D140" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" spans="1:4">
+      <x:c r="A141" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="C141" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="D141" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:4">
+      <x:c r="A142" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="C142" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="D142" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:4">
+      <x:c r="A143" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B143" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="C143" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="D143" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:4">
+      <x:c r="A144" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B144" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="C144" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D144" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" spans="1:4">
+      <x:c r="A145" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B145" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="C145" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="D145" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" spans="1:4">
+      <x:c r="A146" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B146" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="C146" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="D146" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:4">
+      <x:c r="A147" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B147" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="C147" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="D147" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148" spans="1:4">
+      <x:c r="A148" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B148" s="0" t="s">
+        <x:v>299</x:v>
+      </x:c>
+      <x:c r="C148" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="D148" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149" spans="1:4">
+      <x:c r="A149" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B149" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="C149" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="D149" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150" spans="1:4">
+      <x:c r="A150" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B150" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="C150" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="D150" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151" spans="1:4">
+      <x:c r="A151" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B151" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="C151" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="D151" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152" spans="1:4">
+      <x:c r="A152" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B152" s="0" t="s">
+        <x:v>307</x:v>
+      </x:c>
+      <x:c r="C152" s="0" t="s">
+        <x:v>308</x:v>
+      </x:c>
+      <x:c r="D152" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153" spans="1:4">
+      <x:c r="A153" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B153" s="0" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="C153" s="0" t="s">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="D153" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154" spans="1:4">
+      <x:c r="A154" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B154" s="0" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="C154" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="D154" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:4">
+      <x:c r="A155" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B155" s="0" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="C155" s="0" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="D155" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:4">
+      <x:c r="A156" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B156" s="0" t="s">
+        <x:v>315</x:v>
+      </x:c>
+      <x:c r="C156" s="0" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="D156" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:4">
+      <x:c r="A157" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B157" s="0" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="C157" s="0" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="D157" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:4">
+      <x:c r="A158" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B158" s="0" t="s">
+        <x:v>319</x:v>
+      </x:c>
+      <x:c r="C158" s="0" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="D158" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159" spans="1:4">
+      <x:c r="A159" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B159" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="C159" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="D159" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160" spans="1:4">
+      <x:c r="A160" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B160" s="0" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="C160" s="0" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="D160" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="161" spans="1:4">
+      <x:c r="A161" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B161" s="0" t="s">
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="C161" s="0" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="D161" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="162" spans="1:4">
+      <x:c r="A162" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B162" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="C162" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="D162" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="163" spans="1:4">
+      <x:c r="A163" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B163" s="0" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="C163" s="0" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="D163" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="164" spans="1:4">
+      <x:c r="A164" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B164" s="0" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="C164" s="0" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="D164" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="165" spans="1:4">
+      <x:c r="A165" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B165" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="C165" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="D165" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="166" spans="1:4">
+      <x:c r="A166" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B166" s="0" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="C166" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="D166" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="167" spans="1:4">
+      <x:c r="A167" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B167" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C167" s="0" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="D167" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="168" spans="1:4">
+      <x:c r="A168" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B168" s="0" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="C168" s="0" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="D168" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="169" spans="1:4">
+      <x:c r="A169" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B169" s="0" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="C169" s="0" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="D169" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="170" spans="1:4">
+      <x:c r="A170" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B170" s="0" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="C170" s="0" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="D170" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="171" spans="1:4">
+      <x:c r="A171" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B171" s="0" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="C171" s="0" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="D171" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="172" spans="1:4">
+      <x:c r="A172" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B172" s="0" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="C172" s="0" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="D172" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="173" spans="1:4">
+      <x:c r="A173" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B173" s="0" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="C173" s="0" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="D173" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="174" spans="1:4">
+      <x:c r="A174" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B174" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="C174" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="D174" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="175" spans="1:4">
+      <x:c r="A175" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B175" s="0" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="C175" s="0" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="D175" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="176" spans="1:4">
+      <x:c r="A176" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B176" s="0" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="C176" s="0" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="D176" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="177" spans="1:4">
+      <x:c r="A177" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B177" s="0" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="C177" s="0" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="D177" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="178" spans="1:4">
+      <x:c r="A178" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B178" s="0" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="C178" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="D178" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="179" spans="1:4">
+      <x:c r="A179" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B179" s="0" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="C179" s="0" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="D179" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="180" spans="1:4">
+      <x:c r="A180" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B180" s="0" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="C180" s="0" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="D180" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="181" spans="1:4">
+      <x:c r="A181" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B181" s="0" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="C181" s="0" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="D181" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="182" spans="1:4">
+      <x:c r="A182" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B182" s="0" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="C182" s="0" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="D182" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="183" spans="1:4">
+      <x:c r="A183" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B183" s="0" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="C183" s="0" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="D183" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="184" spans="1:4">
+      <x:c r="A184" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B184" s="0" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="C184" s="0" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="D184" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="185" spans="1:4">
+      <x:c r="A185" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B185" s="0" t="s">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="C185" s="0" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="D185" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="186" spans="1:4">
+      <x:c r="A186" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B186" s="0" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="C186" s="0" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="D186" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="187" spans="1:4">
+      <x:c r="A187" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B187" s="0" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="C187" s="0" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="D187" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="188" spans="1:4">
+      <x:c r="A188" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B188" s="0" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="C188" s="0" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="D188" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="189" spans="1:4">
+      <x:c r="A189" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B189" s="0" t="s">
+        <x:v>381</x:v>
+      </x:c>
+      <x:c r="C189" s="0" t="s">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="D189" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="190" spans="1:4">
+      <x:c r="A190" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B190" s="0" t="s">
+        <x:v>383</x:v>
+      </x:c>
+      <x:c r="C190" s="0" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="D190" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="191" spans="1:4">
+      <x:c r="A191" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B191" s="0" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="C191" s="0" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="D191" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="192" spans="1:4">
+      <x:c r="A192" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B192" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="C192" s="0" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="D192" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="193" spans="1:4">
+      <x:c r="A193" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B193" s="0" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="C193" s="0" t="s">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="D193" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="194" spans="1:4">
+      <x:c r="A194" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B194" s="0" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="C194" s="0" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="D194" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="195" spans="1:4">
+      <x:c r="A195" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B195" s="0" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="C195" s="0" t="s">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="D195" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="196" spans="1:4">
+      <x:c r="A196" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B196" s="0" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="C196" s="0" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="D196" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="197" spans="1:4">
+      <x:c r="A197" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B197" s="0" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="C197" s="0" t="s">
+        <x:v>398</x:v>
+      </x:c>
+      <x:c r="D197" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="198" spans="1:4">
+      <x:c r="A198" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B198" s="0" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="C198" s="0" t="s">
+        <x:v>400</x:v>
+      </x:c>
+      <x:c r="D198" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="199" spans="1:4">
+      <x:c r="A199" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B199" s="0" t="s">
+        <x:v>401</x:v>
+      </x:c>
+      <x:c r="C199" s="0" t="s">
+        <x:v>402</x:v>
+      </x:c>
+      <x:c r="D199" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="200" spans="1:4">
+      <x:c r="A200" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B200" s="0" t="s">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="C200" s="0" t="s">
+        <x:v>404</x:v>
+      </x:c>
+      <x:c r="D200" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>